<commit_message>
Se actualiza el controlador de dispositivos y bitácoras para el modal de bitácoras
</commit_message>
<xml_diff>
--- a/src/main/resources/static/FO-GTI-02.xlsx
+++ b/src/main/resources/static/FO-GTI-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\IdeaProjects\inventory-system\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE7CF36F-8324-4880-9496-F2A9C13F03BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D55F485-BDFA-41F0-A72B-C215542533DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>ESTADO</t>
   </si>
@@ -155,9 +155,6 @@
       </rPr>
       <t>07-jun-2016</t>
     </r>
-  </si>
-  <si>
-    <t>Carlos Andres Jimenez Rios</t>
   </si>
   <si>
     <t>EL ABAJO FIRMANTE DE LA PRESENTE ACTA EN CALIDAD DE TRABAJADOR DE POTENCIA Y TECNOLOGIAS INCORPORADAS S.A. BIC. (EN ADELANTE "PTI"), EN VIRTUD DE ESTE INSTRUMENTO REALIZO LAS SIGUIENTES DECLARACIONES Y AUTORIZACIONES:
@@ -614,31 +611,163 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,138 +805,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -899,57 +896,6 @@
             </a14:hiddenLine>
           </a:ext>
         </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76786</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>14654</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>439615</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>55718</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3A45B2B-70E0-0BEA-11C9-539758E58ED5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:biLevel thresh="50000"/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1366324" y="7165731"/>
-          <a:ext cx="2718582" cy="674696"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1250,7 +1196,7 @@
   <dimension ref="B1:J34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="54" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G31" sqref="G31:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1279,42 +1225,42 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="2:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="77"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="78"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="68"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="79"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="11"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
       <c r="J4" s="12" t="s">
         <v>27</v>
       </c>
@@ -1331,140 +1277,140 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="73"/>
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="29"/>
+      <c r="G6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="16"/>
     </row>
     <row r="7" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="80"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="19" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="19" t="s">
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="21"/>
+      <c r="J7" s="31"/>
     </row>
     <row r="8" spans="2:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="2:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
       <c r="I10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="2:10" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="55" t="s">
+      <c r="C12" s="51"/>
+      <c r="D12" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="56"/>
-      <c r="F12" s="25" t="s">
+      <c r="E12" s="51"/>
+      <c r="F12" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="75" t="s">
+      <c r="G12" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="76"/>
-      <c r="I12" s="25" t="s">
+      <c r="H12" s="36"/>
+      <c r="I12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="J12" s="33" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="57"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="27"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
       <c r="F14" s="6"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
@@ -1472,10 +1418,10 @@
       <c r="J14" s="17"/>
     </row>
     <row r="15" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
       <c r="F15" s="6"/>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
@@ -1483,10 +1429,10 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="6"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
@@ -1494,10 +1440,10 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="6"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
@@ -1505,10 +1451,10 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="6"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
@@ -1516,10 +1462,10 @@
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
       <c r="F19" s="6"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
@@ -1527,176 +1473,200 @@
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="48"/>
+      <c r="B20" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="63"/>
     </row>
     <row r="21" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="49"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="66"/>
     </row>
     <row r="22" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="49"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="66"/>
     </row>
     <row r="23" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="51"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="66"/>
     </row>
     <row r="24" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="49"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="51"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="66"/>
     </row>
     <row r="25" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="49"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="66"/>
     </row>
     <row r="26" spans="2:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="52"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="54"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="69"/>
     </row>
     <row r="27" spans="2:10" s="2" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
     </row>
     <row r="28" spans="2:10" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="44"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="60"/>
     </row>
     <row r="29" spans="2:10" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="19" t="s">
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="21"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="25" t="s">
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="29"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="73"/>
     </row>
     <row r="32" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="26"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="31"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="75"/>
     </row>
     <row r="33" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="26"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="31"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="75"/>
     </row>
     <row r="34" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="27"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="F30:J30"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="G31:J34"/>
+    <mergeCell ref="C31:E34"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B20:J26"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="D2:I4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B10:C10"/>
@@ -1713,32 +1683,6 @@
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:J26"/>
-    <mergeCell ref="F30:J30"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="G31:J34"/>
-    <mergeCell ref="C31:E34"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>